<commit_message>
working on llyods based on charlies data
</commit_message>
<xml_diff>
--- a/data/China_Construction_Bank_Data_13-23.xlsx
+++ b/data/China_Construction_Bank_Data_13-23.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caesa/Desktop/CoCo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B0E7D7-1F77-7740-9854-5D570D90DE52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5DC97E-9712-BF47-813C-088DE0EEF10C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="27060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Returns" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>2015Q1</t>
   </si>
@@ -168,9 +168,6 @@
     <t>Note</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>Open</t>
   </si>
   <si>
@@ -180,13 +177,16 @@
     <t>Low</t>
   </si>
   <si>
-    <t>Close</t>
-  </si>
-  <si>
     <t>CET-1 ratio (phase-in)</t>
   </si>
   <si>
     <t>Log-returns without dividends</t>
+  </si>
+  <si>
+    <t>Names Date</t>
+  </si>
+  <si>
+    <t>Price or Bid/Ask Average</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <dimension ref="A1:F2590"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -539,22 +539,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="E1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -54935,7 +54935,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -54944,11 +54944,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="2"/>
+      <c r="A1" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>42</v>

</xml_diff>